<commit_message>
Unit test ok. New Models project. New DataAccess project. Reorganize overall code. ExcelFileManager, GetContact function return a 'Contact' list
</commit_message>
<xml_diff>
--- a/contact.xlsx
+++ b/contact.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUPINFO\STAGE\TonicTeaching\TONIC-certificate-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A162A73F-728A-4C33-8B67-2FA2923E16E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1FF875-94F4-48B3-8BDA-C71655B2DE32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>firstname</t>
   </si>
@@ -43,6 +43,24 @@
   </si>
   <si>
     <t>jeanmarcelle@exemple.com</t>
+  </si>
+  <si>
+    <t>marie</t>
+  </si>
+  <si>
+    <t>janne</t>
+  </si>
+  <si>
+    <t>mariejanne@exemple.com</t>
+  </si>
+  <si>
+    <t>dupont</t>
+  </si>
+  <si>
+    <t>pierre</t>
+  </si>
+  <si>
+    <t>dupontpierre@exemple.com</t>
   </si>
 </sst>
 </file>
@@ -371,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,10 +422,29 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{5B226F8E-EC5D-4ECF-9B05-923E787AECDA}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>